<commit_message>
The second part of the Validation
</commit_message>
<xml_diff>
--- a/datafiles/cbn_MFB_rpt_12345m052087.xlsx
+++ b/datafiles/cbn_MFB_rpt_12345m052087.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saliu\Documents\FOR SAMUEL\NEPTUNE PROJECTS\EFASS-BACK\EfassBack\Efass-BackEnd\datafiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12735" windowHeight="9855" tabRatio="937" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="3570" tabRatio="937" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="300" sheetId="1" r:id="rId1"/>
@@ -46,6 +41,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'300'!$A$1:$F$119</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <oleSize ref="A22:H30"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -55,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="449">
   <si>
     <t>Micro-Finance Bank Code</t>
   </si>
@@ -2470,6 +2466,18 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>hhghg</t>
+  </si>
+  <si>
+    <t>ffdf</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -7069,7 +7077,7 @@
       <c r="C35" s="58"/>
       <c r="D35" s="48">
         <f>'711'!D20</f>
-        <v>7280</v>
+        <v>7946</v>
       </c>
       <c r="E35" s="36"/>
       <c r="F35" s="37"/>
@@ -7162,7 +7170,7 @@
       <c r="D42" s="36"/>
       <c r="E42" s="40">
         <f>SUM(D35:D41)</f>
-        <v>13280</v>
+        <v>13946</v>
       </c>
       <c r="F42" s="37"/>
     </row>
@@ -7223,7 +7231,7 @@
       <c r="E46" s="36"/>
       <c r="F46" s="41">
         <f>E42-E45</f>
-        <v>13147.2</v>
+        <v>13813.2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -7434,7 +7442,7 @@
       <c r="E61" s="64"/>
       <c r="F61" s="65">
         <f>F60+F50+F46+F33+F27+F25+F17</f>
-        <v>35871.199999999997</v>
+        <v>36537.199999999997</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -8231,7 +8239,7 @@
   </sheetPr>
   <dimension ref="A1:IW24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -8469,9 +8477,9 @@
         <v>232</v>
       </c>
       <c r="C20" s="675"/>
-      <c r="D20" s="365">
+      <c r="D20" s="365" t="str">
         <f>IF(D19+D18+D12='300'!E42,D19+D18+D12,"Check Rules!!!")</f>
-        <v>13280</v>
+        <v>Check Rules!!!</v>
       </c>
       <c r="E20" s="157"/>
     </row>
@@ -8496,12 +8504,12 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="93" t="str">
         <f>IF(D20="Check Rules!!!",D20,"…………………………………………………..")</f>
-        <v>…………………………………………………..</v>
+        <v>Check Rules!!!</v>
       </c>
       <c r="B23" s="90"/>
       <c r="C23" s="650" t="str">
         <f>A23</f>
-        <v>…………………………………………………..</v>
+        <v>Check Rules!!!</v>
       </c>
       <c r="D23" s="650"/>
       <c r="E23" s="158"/>
@@ -8558,8 +8566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW195"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A2" zoomScale="84" zoomScaleNormal="70" zoomScalePageLayoutView="84" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="70" zoomScalePageLayoutView="84" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9033,7 +9041,9 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="391"/>
-      <c r="B20" s="392"/>
+      <c r="B20" s="392" t="s">
+        <v>448</v>
+      </c>
       <c r="C20" s="393"/>
       <c r="D20" s="394"/>
       <c r="E20" s="237"/>
@@ -9056,7 +9066,9 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="401"/>
-      <c r="B21" s="402"/>
+      <c r="B21" s="402">
+        <v>55</v>
+      </c>
       <c r="C21" s="403"/>
       <c r="D21" s="404"/>
       <c r="E21" s="404"/>
@@ -13120,8 +13132,8 @@
   </sheetPr>
   <dimension ref="A1:IW30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D24"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13266,8 +13278,12 @@
         <v>283</v>
       </c>
       <c r="B12" s="683"/>
-      <c r="C12" s="415"/>
-      <c r="D12" s="416"/>
+      <c r="C12" s="415">
+        <v>123</v>
+      </c>
+      <c r="D12" s="416">
+        <v>121</v>
+      </c>
       <c r="E12" s="417" t="e">
         <f t="shared" ref="E12:E24" si="0">D12/$D$25</f>
         <v>#VALUE!</v>
@@ -13424,7 +13440,7 @@
       <c r="B25" s="686"/>
       <c r="C25" s="426">
         <f>SUM(C12:C24)</f>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="D25" s="427" t="str">
         <f>IF(SUM(D12:D24)='300'!E42,SUM(D12:D24),"Check Rules!!!")</f>
@@ -13526,7 +13542,7 @@
   </sheetPr>
   <dimension ref="A1:IW44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -13760,9 +13776,9 @@
         <f>SUM(C15:H15)</f>
         <v>7280</v>
       </c>
-      <c r="J15" s="449">
+      <c r="J15" s="449" t="e">
         <f>I15/$I$33*100</f>
-        <v>54.819277108433738</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -13818,9 +13834,9 @@
         <f>SUM(C18:H18)</f>
         <v>6000</v>
       </c>
-      <c r="J18" s="449">
+      <c r="J18" s="449" t="e">
         <f>I18/$I$33*100</f>
-        <v>45.180722891566269</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -13872,9 +13888,9 @@
         <f>SUM(C21:H21)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="449">
+      <c r="J21" s="449" t="e">
         <f>I21/$I$33*100</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -13926,9 +13942,9 @@
         <f>SUM(C24:H24)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="449">
+      <c r="J24" s="449" t="e">
         <f>I24/$I$33*100</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -13980,9 +13996,9 @@
         <f>SUM(C27:H27)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="449">
+      <c r="J27" s="449" t="e">
         <f>I27/$I$33*100</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -14034,9 +14050,9 @@
         <f>SUM(C30:H30)</f>
         <v>0</v>
       </c>
-      <c r="J30" s="452">
+      <c r="J30" s="452" t="e">
         <f>I30/$I$33*100</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -14120,13 +14136,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I33" s="457">
+      <c r="I33" s="457" t="str">
         <f>IF(I15+I18+I21+I24+I27+I30='300'!E42,I15+I18+I21+I24+I27+I30,"Check Rules!!!")</f>
-        <v>13280</v>
-      </c>
-      <c r="J33" s="458">
+        <v>Check Rules!!!</v>
+      </c>
+      <c r="J33" s="458" t="e">
         <f>J15+J18+J21+J24+J27+J30</f>
-        <v>100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="440" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14156,14 +14172,14 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="93" t="str">
         <f>IF(I33="Check Rules!!!",I33,"……………………………………………………..")</f>
-        <v>……………………………………………………..</v>
+        <v>Check Rules!!!</v>
       </c>
       <c r="B36" s="437"/>
       <c r="E36" s="462"/>
       <c r="F36" s="462"/>
       <c r="G36" s="694" t="str">
         <f>A36</f>
-        <v>……………………………………………………..</v>
+        <v>Check Rules!!!</v>
       </c>
       <c r="H36" s="694"/>
       <c r="I36" s="462"/>
@@ -14323,7 +14339,7 @@
   </sheetPr>
   <dimension ref="A1:IW23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -15102,7 +15118,7 @@
   </sheetPr>
   <dimension ref="A1:IW52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
@@ -15552,7 +15568,7 @@
   </sheetPr>
   <dimension ref="A1:IW40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -24423,8 +24439,8 @@
   </sheetPr>
   <dimension ref="A1:IW24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24586,7 +24602,7 @@
       </c>
       <c r="E12" s="311">
         <f t="shared" ref="E12:E19" si="0">D12/$D$20</f>
-        <v>1</v>
+        <v>0.91618424364460105</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -24596,11 +24612,15 @@
       <c r="B13" s="313" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="314"/>
-      <c r="D13" s="73"/>
+      <c r="C13" s="314">
+        <v>90</v>
+      </c>
+      <c r="D13" s="73">
+        <v>666</v>
+      </c>
       <c r="E13" s="315">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3815756355398938E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -24694,11 +24714,11 @@
       </c>
       <c r="C20" s="324">
         <f>SUM(C12:C19)</f>
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="D20" s="325">
         <f>SUM(D12:D19)</f>
-        <v>7280</v>
+        <v>7946</v>
       </c>
       <c r="E20" s="326">
         <f>SUM(E12:E19)</f>
@@ -24763,8 +24783,8 @@
   </sheetPr>
   <dimension ref="A1:IW44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25005,21 +25025,35 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="235"/>
-      <c r="B18" s="338"/>
-      <c r="C18" s="339"/>
-      <c r="D18" s="340"/>
-      <c r="E18" s="341"/>
+      <c r="B18" s="338" t="s">
+        <v>445</v>
+      </c>
+      <c r="C18" s="339">
+        <v>44116</v>
+      </c>
+      <c r="D18" s="340">
+        <v>4</v>
+      </c>
+      <c r="E18" s="341">
+        <v>544</v>
+      </c>
       <c r="F18" s="341"/>
-      <c r="G18" s="342"/>
+      <c r="G18" s="342" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="240"/>
       <c r="B19" s="343"/>
       <c r="C19" s="344"/>
-      <c r="D19" s="345"/>
+      <c r="D19" s="345" t="s">
+        <v>446</v>
+      </c>
       <c r="E19" s="346"/>
       <c r="F19" s="346"/>
-      <c r="G19" s="347"/>
+      <c r="G19" s="347">
+        <v>555</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="240"/>

</xml_diff>